<commit_message>
Unify analysis scale to 0-1500m corridor (near=0-300m, far=750-1500m)
- config.py: extend BUFFER_DISTANCES to 1500m, add NEAR_DISTANCE_MAX/FAR_DISTANCE_MIN/MAX_CORRIDOR_DISTANCE constants
- Script 02: buffers now 30-1500m (24 rings), import MAX_CORRIDOR_DISTANCE for plot title
- Script 05: near threshold 60m->300m, far threshold 800m->750m, import unified constants
- Re-ran Script 02: regenerated all 12 Gradient_Month_XX.xlsx + All_Months_Gradient.xlsx + 27 PNGs
- Re-ran Script 05: regenerated Seasonal_Metrics_Summary.csv + 5 PNGs
- README/OPERATION_GUIDE: buffer range updated 1000m->1500m

All scripts now share one consistent analysis scale matching Script 07 riverside corridor.
</commit_message>
<xml_diff>
--- a/Data/Gradient_Month_01.xlsx
+++ b/Data/Gradient_Month_01.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -933,6 +933,131 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1100</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3.951002359390259</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.281787157058716</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-0.6831467747688293</v>
+      </c>
+      <c r="E21" t="n">
+        <v>9.308746337890625</v>
+      </c>
+      <c r="F21" t="n">
+        <v>18476</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1200</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.904142141342163</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.283282518386841</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-0.9052648544311523</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10.12545680999756</v>
+      </c>
+      <c r="F22" t="n">
+        <v>18568</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.842416048049927</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.282211780548096</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-0.9531055688858032</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10.13229084014893</v>
+      </c>
+      <c r="F23" t="n">
+        <v>18438</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1400</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3.818761587142944</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.266582608222961</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.8215433955192566</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8.560379028320312</v>
+      </c>
+      <c r="F24" t="n">
+        <v>18366</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B25" t="n">
+        <v>3.787439107894897</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1.304946541786194</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-1.019741058349609</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10.73371887207031</v>
+      </c>
+      <c r="F25" t="n">
+        <v>18392</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>